<commit_message>
Created example VGG search using CIFAR10.
</commit_message>
<xml_diff>
--- a/log/VGG_CIFAR10_20240324.xlsx
+++ b/log/VGG_CIFAR10_20240324.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -868,6 +868,391 @@
         <v>0.1027999967336655</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>3</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>128</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>6</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.7784000039100647</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.7749999761581421</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>3</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>128</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>6</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.7633000016212463</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.7513999938964844</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>20</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.163987255</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.102922781</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.133724907</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.010547912</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.087016579</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2.96260662</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-0.111799513</v>
+      </c>
+      <c r="S8" t="n">
+        <v>128</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-0.001166751</v>
+      </c>
+      <c r="U8" t="n">
+        <v>6</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.102167731</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.8555999994277954</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.8532000184059143</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>20</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>128</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>6</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.7573999762535095</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.7531999945640564</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>20</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.163987255</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.102922781</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.133724907</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.010547912</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.087016579</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2.96260662</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-0.111799513</v>
+      </c>
+      <c r="S10" t="n">
+        <v>128</v>
+      </c>
+      <c r="T10" t="n">
+        <v>-0.001166751</v>
+      </c>
+      <c r="U10" t="n">
+        <v>6</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.102167731</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.8578000068664551</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.843999981880188</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>